<commit_message>
Made a bunch of changes
</commit_message>
<xml_diff>
--- a/Replication Package/Code and Data/(2) Regressions/Output Data (New Pre Covid Detrended ED)/eq_coefficients_new_model_pre_covid.xlsx
+++ b/Replication Package/Code and Data/(2) Regressions/Output Data (New Pre Covid Detrended ED)/eq_coefficients_new_model_pre_covid.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,6 +453,11 @@
           <t>se</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>pvalue</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -466,6 +471,9 @@
       <c r="C2" t="n">
         <v>0.2070124340894315</v>
       </c>
+      <c r="D2" t="n">
+        <v>0.1290234611231549</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -479,6 +487,9 @@
       <c r="C3" t="n">
         <v>0.1067642120238665</v>
       </c>
+      <c r="D3" t="n">
+        <v>0.3002085914212871</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -492,6 +503,9 @@
       <c r="C4" t="n">
         <v>0.1042295436735185</v>
       </c>
+      <c r="D4" t="n">
+        <v>0.2220009610422526</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -505,6 +519,9 @@
       <c r="C5" t="n">
         <v>0.1045921555929096</v>
       </c>
+      <c r="D5" t="n">
+        <v>0.1446924608367512</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -518,6 +535,9 @@
       <c r="C6" t="n">
         <v>0.1031040983299641</v>
       </c>
+      <c r="D6" t="n">
+        <v>0.7931830271606073</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -531,6 +551,9 @@
       <c r="C7" t="n">
         <v>0.1473758634096519</v>
       </c>
+      <c r="D7" t="n">
+        <v>0.01931924298648724</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -544,6 +567,9 @@
       <c r="C8" t="n">
         <v>0.1553932443057404</v>
       </c>
+      <c r="D8" t="n">
+        <v>0.7310042812157449</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -557,6 +583,9 @@
       <c r="C9" t="n">
         <v>0.1634909088799052</v>
       </c>
+      <c r="D9" t="n">
+        <v>0.2792822672512854</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -570,6 +599,9 @@
       <c r="C10" t="n">
         <v>0.1599606189577532</v>
       </c>
+      <c r="D10" t="n">
+        <v>0.7456121300667227</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -583,6 +615,9 @@
       <c r="C11" t="n">
         <v>0.07979985871985025</v>
       </c>
+      <c r="D11" t="n">
+        <v>0.851843368544956</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -596,6 +631,9 @@
       <c r="C12" t="n">
         <v>2.290832346379283</v>
       </c>
+      <c r="D12" t="n">
+        <v>0.0608373940281397</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -609,6 +647,9 @@
       <c r="C13" t="n">
         <v>3.988810121879009</v>
       </c>
+      <c r="D13" t="n">
+        <v>0.9762627204220351</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -622,6 +663,9 @@
       <c r="C14" t="n">
         <v>4.036121648430077</v>
       </c>
+      <c r="D14" t="n">
+        <v>0.1847361598184509</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -635,6 +679,9 @@
       <c r="C15" t="n">
         <v>2.550059993216784</v>
       </c>
+      <c r="D15" t="n">
+        <v>0.4675677972722876</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -648,6 +695,9 @@
       <c r="C16" t="n">
         <v>0.08404508422231663</v>
       </c>
+      <c r="D16" t="n">
+        <v>0.6226180440369955</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -661,6 +711,9 @@
       <c r="C17" t="n">
         <v>0.08542246289564952</v>
       </c>
+      <c r="D17" t="n">
+        <v>0.9277040593429429</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -674,6 +727,9 @@
       <c r="C18" t="n">
         <v>0.08109840483561849</v>
       </c>
+      <c r="D18" t="n">
+        <v>0.6670376289183653</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -687,6 +743,9 @@
       <c r="C19" t="n">
         <v>0.0700365940104134</v>
       </c>
+      <c r="D19" t="n">
+        <v>0.7306182199557716</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -700,6 +759,9 @@
       <c r="C20" t="n">
         <v>12.53777300128307</v>
       </c>
+      <c r="D20" t="n">
+        <v>0.9061852317161634</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -713,6 +775,9 @@
       <c r="C21" t="n">
         <v>22.07642078836592</v>
       </c>
+      <c r="D21" t="n">
+        <v>0.2623195462746581</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -726,6 +791,9 @@
       <c r="C22" t="n">
         <v>22.44529177552516</v>
       </c>
+      <c r="D22" t="n">
+        <v>0.2454381904917984</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -738,6 +806,9 @@
       </c>
       <c r="C23" t="n">
         <v>13.04063890586476</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.5973951366002259</v>
       </c>
     </row>
   </sheetData>
@@ -751,7 +822,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -775,6 +846,11 @@
           <t>se</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>pvalue</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -788,6 +864,9 @@
       <c r="C2" t="n">
         <v>1.107274434386906</v>
       </c>
+      <c r="D2" t="n">
+        <v>0.0003162805065090288</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -801,6 +880,9 @@
       <c r="C3" t="n">
         <v>0.08811083674314943</v>
       </c>
+      <c r="D3" t="n">
+        <v>0.7323874358597695</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -814,6 +896,9 @@
       <c r="C4" t="n">
         <v>0.08423686466845988</v>
       </c>
+      <c r="D4" t="n">
+        <v>0.49391430881917</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -827,6 +912,9 @@
       <c r="C5" t="n">
         <v>0.0826425806481708</v>
       </c>
+      <c r="D5" t="n">
+        <v>0.003598497022740576</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -840,6 +928,9 @@
       <c r="C6" t="n">
         <v>0.08672326249814835</v>
       </c>
+      <c r="D6" t="n">
+        <v>0.003880380508392888</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -853,6 +944,9 @@
       <c r="C7" t="n">
         <v>16.85169152862024</v>
       </c>
+      <c r="D7" t="n">
+        <v>0.02163957395632394</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -866,6 +960,9 @@
       <c r="C8" t="n">
         <v>23.33815517252609</v>
       </c>
+      <c r="D8" t="n">
+        <v>8.239817215566001e-06</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -879,6 +976,9 @@
       <c r="C9" t="n">
         <v>25.50455176969453</v>
       </c>
+      <c r="D9" t="n">
+        <v>0.1421789981415316</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -892,6 +992,9 @@
       <c r="C10" t="n">
         <v>25.59333074672177</v>
       </c>
+      <c r="D10" t="n">
+        <v>0.002806223942581709</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -905,6 +1008,9 @@
       <c r="C11" t="n">
         <v>18.6737895074883</v>
       </c>
+      <c r="D11" t="n">
+        <v>0.00173225779679854</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -918,6 +1024,9 @@
       <c r="C12" t="n">
         <v>0.7190811354684982</v>
       </c>
+      <c r="D12" t="n">
+        <v>2.652903284271935e-07</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -931,6 +1040,9 @@
       <c r="C13" t="n">
         <v>1.034466677036626</v>
       </c>
+      <c r="D13" t="n">
+        <v>0.07241849061627345</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -944,6 +1056,9 @@
       <c r="C14" t="n">
         <v>1.014433579134348</v>
       </c>
+      <c r="D14" t="n">
+        <v>0.9454398639911507</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -957,6 +1072,9 @@
       <c r="C15" t="n">
         <v>0.982265233365745</v>
       </c>
+      <c r="D15" t="n">
+        <v>0.3585449778807103</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -969,6 +1087,9 @@
       </c>
       <c r="C16" t="n">
         <v>0.8037532099556828</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.009287613265408437</v>
       </c>
     </row>
   </sheetData>
@@ -982,7 +1103,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1006,6 +1127,11 @@
           <t>se</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>pvalue</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1019,6 +1145,9 @@
       <c r="C2" t="n">
         <v>0.1580048776318225</v>
       </c>
+      <c r="D2" t="n">
+        <v>0.5010960927306609</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1032,6 +1161,9 @@
       <c r="C3" t="n">
         <v>0.06357949463548257</v>
       </c>
+      <c r="D3" t="n">
+        <v>0.02538533875937854</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1045,6 +1177,9 @@
       <c r="C4" t="n">
         <v>0.1077454260836043</v>
       </c>
+      <c r="D4" t="n">
+        <v>0.6953909609254256</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1058,6 +1193,9 @@
       <c r="C5" t="n">
         <v>0.102207730605524</v>
       </c>
+      <c r="D5" t="n">
+        <v>0.08810637587206394</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1071,6 +1209,9 @@
       <c r="C6" t="n">
         <v>0.1019737278549629</v>
       </c>
+      <c r="D6" t="n">
+        <v>0.02735932922402307</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1084,6 +1225,9 @@
       <c r="C7" t="n">
         <v>0.09731760162507391</v>
       </c>
+      <c r="D7" t="n">
+        <v>0.2452276902447852</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1097,6 +1241,9 @@
       <c r="C8" t="n">
         <v>0.09354206897094307</v>
       </c>
+      <c r="D8" t="n">
+        <v>0.0001448686781584385</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1110,6 +1257,9 @@
       <c r="C9" t="n">
         <v>0.1082706982209676</v>
       </c>
+      <c r="D9" t="n">
+        <v>0.1073587853777496</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1123,6 +1273,9 @@
       <c r="C10" t="n">
         <v>0.1073369809267438</v>
       </c>
+      <c r="D10" t="n">
+        <v>0.7228603072823396</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1136,6 +1289,9 @@
       <c r="C11" t="n">
         <v>0.1103332233696892</v>
       </c>
+      <c r="D11" t="n">
+        <v>0.7458551455260674</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1149,6 +1305,9 @@
       <c r="C12" t="n">
         <v>0.1037433963052754</v>
       </c>
+      <c r="D12" t="n">
+        <v>0.637312235973623</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1162,6 +1321,9 @@
       <c r="C13" t="n">
         <v>0.002680931462540892</v>
       </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1175,6 +1337,9 @@
       <c r="C14" t="n">
         <v>0.009930362206725133</v>
       </c>
+      <c r="D14" t="n">
+        <v>0.9523798043850926</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1188,6 +1353,9 @@
       <c r="C15" t="n">
         <v>0.009479596497237459</v>
       </c>
+      <c r="D15" t="n">
+        <v>0.1207433474388797</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1201,6 +1369,9 @@
       <c r="C16" t="n">
         <v>0.009429193235158062</v>
       </c>
+      <c r="D16" t="n">
+        <v>0.02602729997513364</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1214,6 +1385,9 @@
       <c r="C17" t="n">
         <v>0.008964357977177279</v>
       </c>
+      <c r="D17" t="n">
+        <v>0.29966872524489</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1227,6 +1401,9 @@
       <c r="C18" t="n">
         <v>0.03571281864225156</v>
       </c>
+      <c r="D18" t="n">
+        <v>0.002404929925602373</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1240,6 +1417,9 @@
       <c r="C19" t="n">
         <v>0.03930697970864193</v>
       </c>
+      <c r="D19" t="n">
+        <v>0.6930418784685828</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1253,6 +1433,9 @@
       <c r="C20" t="n">
         <v>0.03782650204728617</v>
       </c>
+      <c r="D20" t="n">
+        <v>0.9806205159169896</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1266,6 +1449,9 @@
       <c r="C21" t="n">
         <v>0.03698085522277976</v>
       </c>
+      <c r="D21" t="n">
+        <v>0.9051182364921984</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1279,6 +1465,9 @@
       <c r="C22" t="n">
         <v>0.03535046763551423</v>
       </c>
+      <c r="D22" t="n">
+        <v>0.3115380699618699</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1292,6 +1481,9 @@
       <c r="C23" t="n">
         <v>0.02055991727946756</v>
       </c>
+      <c r="D23" t="n">
+        <v>8.614829429820503e-07</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1305,6 +1497,9 @@
       <c r="C24" t="n">
         <v>0.02161439696437044</v>
       </c>
+      <c r="D24" t="n">
+        <v>0.1294541507853844</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1318,6 +1513,9 @@
       <c r="C25" t="n">
         <v>0.02011368089680392</v>
       </c>
+      <c r="D25" t="n">
+        <v>0.9721489187917656</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1331,6 +1529,9 @@
       <c r="C26" t="n">
         <v>0.02173686745994822</v>
       </c>
+      <c r="D26" t="n">
+        <v>0.1340809643009924</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1343,6 +1544,9 @@
       </c>
       <c r="C27" t="n">
         <v>0.02177109222214522</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.2828192680549182</v>
       </c>
     </row>
   </sheetData>
@@ -1356,7 +1560,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1380,6 +1584,11 @@
           <t>se</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>pvalue</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1393,6 +1602,9 @@
       <c r="C2" t="n">
         <v>0.0951182906203049</v>
       </c>
+      <c r="D2" t="n">
+        <v>0.001870565130419166</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1406,6 +1618,9 @@
       <c r="C3" t="n">
         <v>0.09757633880614289</v>
       </c>
+      <c r="D3" t="n">
+        <v>0.0223415990145619</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1419,6 +1634,9 @@
       <c r="C4" t="n">
         <v>0.09682467247285041</v>
       </c>
+      <c r="D4" t="n">
+        <v>0.07192015529401363</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1432,6 +1650,9 @@
       <c r="C5" t="n">
         <v>0.07262195790613224</v>
       </c>
+      <c r="D5" t="n">
+        <v>0.1127638405524429</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1445,6 +1666,9 @@
       <c r="C6" t="n">
         <v>0.1441256677691466</v>
       </c>
+      <c r="D6" t="n">
+        <v>3.077538224260934e-13</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1458,6 +1682,9 @@
       <c r="C7" t="n">
         <v>0.228701389125017</v>
       </c>
+      <c r="D7" t="n">
+        <v>0.04263410282467461</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1471,6 +1698,9 @@
       <c r="C8" t="n">
         <v>0.2321564042407155</v>
       </c>
+      <c r="D8" t="n">
+        <v>0.94077935258546</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1484,6 +1714,9 @@
       <c r="C9" t="n">
         <v>0.2309949907647698</v>
       </c>
+      <c r="D9" t="n">
+        <v>0.5602247091789718</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1497,6 +1730,9 @@
       <c r="C10" t="n">
         <v>0.175067039131841</v>
       </c>
+      <c r="D10" t="n">
+        <v>0.03324323423663222</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1510,6 +1746,9 @@
       <c r="C11" t="n">
         <v>0.01267003627366312</v>
       </c>
+      <c r="D11" t="n">
+        <v>0.003431909069939953</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1523,6 +1762,9 @@
       <c r="C12" t="n">
         <v>0.01328191475155815</v>
       </c>
+      <c r="D12" t="n">
+        <v>4.689804100621586e-12</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1536,6 +1778,9 @@
       <c r="C13" t="n">
         <v>0.01628982341616244</v>
       </c>
+      <c r="D13" t="n">
+        <v>0.9569558931800684</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1549,6 +1794,9 @@
       <c r="C14" t="n">
         <v>0.01622726141409656</v>
       </c>
+      <c r="D14" t="n">
+        <v>0.6939145477893458</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1561,6 +1809,9 @@
       </c>
       <c r="C15" t="n">
         <v>0.01613670793619325</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.1353955003801646</v>
       </c>
     </row>
   </sheetData>
@@ -1574,7 +1825,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1598,6 +1849,11 @@
           <t>se</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>pvalue</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1611,6 +1867,9 @@
       <c r="C2" t="n">
         <v>0.09450957064594666</v>
       </c>
+      <c r="D2" t="n">
+        <v>5.773159728050814e-15</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1624,6 +1883,9 @@
       <c r="C3" t="n">
         <v>0.1235893596708862</v>
       </c>
+      <c r="D3" t="n">
+        <v>0.7143722986940217</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1637,6 +1899,9 @@
       <c r="C4" t="n">
         <v>0.1223785151297301</v>
       </c>
+      <c r="D4" t="n">
+        <v>0.1070141664693789</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1650,6 +1915,9 @@
       <c r="C5" t="n">
         <v>0.08857715554601048</v>
       </c>
+      <c r="D5" t="n">
+        <v>0.7146294533782727</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1663,6 +1931,9 @@
       <c r="C6" t="n">
         <v>0.007909922050021397</v>
       </c>
+      <c r="D6" t="n">
+        <v>0.0003383407290487028</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1676,6 +1947,9 @@
       <c r="C7" t="n">
         <v>0.008326497815770184</v>
       </c>
+      <c r="D7" t="n">
+        <v>0.2351671397604802</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1689,6 +1963,9 @@
       <c r="C8" t="n">
         <v>0.00837788894632824</v>
       </c>
+      <c r="D8" t="n">
+        <v>0.1383835634834001</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1702,6 +1979,9 @@
       <c r="C9" t="n">
         <v>0.008386181270502406</v>
       </c>
+      <c r="D9" t="n">
+        <v>0.9482586225333776</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1714,6 +1994,9 @@
       </c>
       <c r="C10" t="n">
         <v>0.008231831697973133</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.8719376760419115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>